<commit_message>
Remove 100.0 from conflict matrix
</commit_message>
<xml_diff>
--- a/conflictMatrices/conflict-matrix-v0.7.xlsx
+++ b/conflictMatrices/conflict-matrix-v0.7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerjan\Workshop\TrafficLightController\conflictMatrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABF1BE7-9DC8-4E1D-B7A0-A294A54CC936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D286574-8967-4486-B1A5-199BE134328A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="225" yWindow="360" windowWidth="25770" windowHeight="20505" xr2:uid="{DF24C662-5795-7044-AEEE-A0FB25F67B06}"/>
+    <workbookView xWindow="-25320" yWindow="-2400" windowWidth="25440" windowHeight="15990" activeTab="1" xr2:uid="{DF24C662-5795-7044-AEEE-A0FB25F67B06}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="2" r:id="rId1"/>
@@ -506,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55E7849-500F-49F3-B09F-3DC7DC01D1AC}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -746,20 +746,20 @@
         <v>99</v>
       </c>
       <c r="B29">
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
-        <v>100</v>
-      </c>
-      <c r="B30">
-        <v>1.5</v>
+        <v>152</v>
+      </c>
+      <c r="B30" s="12">
+        <v>1000000</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B31" s="12">
         <v>1000000</v>
@@ -767,17 +767,9 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B32" s="12">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
-        <v>160</v>
-      </c>
-      <c r="B33" s="12">
         <v>1000000</v>
       </c>
     </row>
@@ -788,19 +780,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B482FAD3-CCB3-9E48-B087-47D1B142F0B2}">
-  <dimension ref="A1:AH33"/>
+  <dimension ref="A1:AG32"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection sqref="A1:A33"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="34" width="9.625" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="10.875" style="1"/>
+    <col min="1" max="33" width="9.625" style="1" customWidth="1"/>
+    <col min="34" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
         <v>1.1000000000000001</v>
       </c>
@@ -892,19 +882,16 @@
         <v>99</v>
       </c>
       <c r="AE1" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF1" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG1" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH1" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>2.1</v>
       </c>
@@ -996,19 +983,16 @@
         <v>99</v>
       </c>
       <c r="AE2" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF2" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG2" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH2" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>5.0999999999999996</v>
       </c>
@@ -1100,19 +1084,16 @@
         <v>99</v>
       </c>
       <c r="AE3" s="8">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF3" s="8">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG3" s="8">
-        <v>154</v>
-      </c>
-      <c r="AH3" s="8">
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>6.1</v>
       </c>
@@ -1204,19 +1185,16 @@
         <v>99</v>
       </c>
       <c r="AE4" s="8">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF4" s="8">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG4" s="8">
-        <v>154</v>
-      </c>
-      <c r="AH4" s="8">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>7.1</v>
       </c>
@@ -1308,19 +1286,16 @@
         <v>99</v>
       </c>
       <c r="AE5" s="8">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF5" s="8">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG5" s="8">
-        <v>154</v>
-      </c>
-      <c r="AH5" s="8">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>8.1</v>
       </c>
@@ -1412,19 +1387,16 @@
         <v>99</v>
       </c>
       <c r="AE6" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF6" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG6" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH6" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>9.1</v>
       </c>
@@ -1516,19 +1488,16 @@
         <v>99</v>
       </c>
       <c r="AE7" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF7" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG7" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH7" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>10.1</v>
       </c>
@@ -1620,19 +1589,16 @@
         <v>99</v>
       </c>
       <c r="AE8" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF8" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG8" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH8" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>11.1</v>
       </c>
@@ -1724,19 +1690,16 @@
         <v>99</v>
       </c>
       <c r="AE9" s="8">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF9" s="8">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG9" s="8">
-        <v>154</v>
-      </c>
-      <c r="AH9" s="8">
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>12.1</v>
       </c>
@@ -1828,19 +1791,16 @@
         <v>99</v>
       </c>
       <c r="AE10" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF10" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG10" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH10" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>86.1</v>
       </c>
@@ -1932,19 +1892,16 @@
         <v>99</v>
       </c>
       <c r="AE11" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF11" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG11" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH11" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>35.1</v>
       </c>
@@ -2036,19 +1993,16 @@
         <v>99</v>
       </c>
       <c r="AE12" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF12" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG12" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH12" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>26.1</v>
       </c>
@@ -2140,19 +2094,16 @@
         <v>99</v>
       </c>
       <c r="AE13" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF13" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG13" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH13" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>36.200000000000003</v>
       </c>
@@ -2244,19 +2195,16 @@
         <v>99</v>
       </c>
       <c r="AE14" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF14" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG14" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH14" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>88.1</v>
       </c>
@@ -2348,19 +2296,16 @@
         <v>99</v>
       </c>
       <c r="AE15" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF15" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG15" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH15" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>37.200000000000003</v>
       </c>
@@ -2452,19 +2397,16 @@
         <v>99</v>
       </c>
       <c r="AE16" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF16" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG16" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH16" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>28.1</v>
       </c>
@@ -2556,19 +2498,16 @@
         <v>99</v>
       </c>
       <c r="AE17" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF17" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG17" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH17" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>38.200000000000003</v>
       </c>
@@ -2660,19 +2599,16 @@
         <v>99</v>
       </c>
       <c r="AE18" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF18" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG18" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH18" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>31.2</v>
       </c>
@@ -2764,19 +2700,16 @@
         <v>99</v>
       </c>
       <c r="AE19" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF19" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG19" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH19" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>22</v>
       </c>
@@ -2868,19 +2801,16 @@
         <v>99</v>
       </c>
       <c r="AE20" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF20" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG20" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH20" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>32.200000000000003</v>
       </c>
@@ -2972,19 +2902,16 @@
         <v>99</v>
       </c>
       <c r="AE21" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF21" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG21" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH21" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>35.200000000000003</v>
       </c>
@@ -3076,19 +3003,16 @@
         <v>99</v>
       </c>
       <c r="AE22" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF22" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG22" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH22" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>36.1</v>
       </c>
@@ -3180,19 +3104,16 @@
         <v>99</v>
       </c>
       <c r="AE23" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF23" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG23" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH23" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>37.1</v>
       </c>
@@ -3284,19 +3205,16 @@
         <v>99</v>
       </c>
       <c r="AE24" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF24" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG24" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH24" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>38.1</v>
       </c>
@@ -3388,19 +3306,16 @@
         <v>99</v>
       </c>
       <c r="AE25" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF25" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG25" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH25" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>31.1</v>
       </c>
@@ -3492,19 +3407,16 @@
         <v>99</v>
       </c>
       <c r="AE26" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF26" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG26" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH26" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>32.1</v>
       </c>
@@ -3596,19 +3508,16 @@
         <v>99</v>
       </c>
       <c r="AE27" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF27" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG27" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH27" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>42</v>
       </c>
@@ -3700,19 +3609,16 @@
         <v>99</v>
       </c>
       <c r="AE28" s="11">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF28" s="11">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG28" s="11">
-        <v>154</v>
-      </c>
-      <c r="AH28" s="11">
         <v>160</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>99</v>
       </c>
@@ -3803,22 +3709,19 @@
       <c r="AD29" s="10">
         <v>99</v>
       </c>
-      <c r="AE29" s="11">
-        <v>100</v>
+      <c r="AE29" s="8">
+        <v>152</v>
       </c>
       <c r="AF29" s="8">
+        <v>154</v>
+      </c>
+      <c r="AG29" s="8">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
         <v>152</v>
-      </c>
-      <c r="AG29" s="8">
-        <v>154</v>
-      </c>
-      <c r="AH29" s="8">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
-        <v>100</v>
       </c>
       <c r="B30" s="11">
         <v>1.1000000000000001</v>
@@ -3904,25 +3807,22 @@
       <c r="AC30" s="11">
         <v>42</v>
       </c>
-      <c r="AD30" s="11">
+      <c r="AD30" s="8">
         <v>99</v>
       </c>
       <c r="AE30" s="10">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF30" s="8">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG30" s="8">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
         <v>154</v>
-      </c>
-      <c r="AH30" s="8">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
-        <v>152</v>
       </c>
       <c r="B31" s="11">
         <v>1.1000000000000001</v>
@@ -4012,21 +3912,18 @@
         <v>99</v>
       </c>
       <c r="AE31" s="8">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF31" s="10">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG31" s="8">
-        <v>154</v>
-      </c>
-      <c r="AH31" s="8">
         <v>160</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B32" s="11">
         <v>1.1000000000000001</v>
@@ -4116,119 +4013,12 @@
         <v>99</v>
       </c>
       <c r="AE32" s="8">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="AF32" s="8">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AG32" s="10">
-        <v>154</v>
-      </c>
-      <c r="AH32" s="8">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
-        <v>160</v>
-      </c>
-      <c r="B33" s="11">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C33" s="11">
-        <v>2.1</v>
-      </c>
-      <c r="D33" s="8">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="E33" s="8">
-        <v>6.1</v>
-      </c>
-      <c r="F33" s="8">
-        <v>7.1</v>
-      </c>
-      <c r="G33" s="11">
-        <v>8.1</v>
-      </c>
-      <c r="H33" s="11">
-        <v>9.1</v>
-      </c>
-      <c r="I33" s="11">
-        <v>10.1</v>
-      </c>
-      <c r="J33" s="8">
-        <v>11.1</v>
-      </c>
-      <c r="K33" s="11">
-        <v>12.1</v>
-      </c>
-      <c r="L33" s="11">
-        <v>86.1</v>
-      </c>
-      <c r="M33" s="11">
-        <v>35.1</v>
-      </c>
-      <c r="N33" s="11">
-        <v>26.1</v>
-      </c>
-      <c r="O33" s="11">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="P33" s="11">
-        <v>88.1</v>
-      </c>
-      <c r="Q33" s="11">
-        <v>37.200000000000003</v>
-      </c>
-      <c r="R33" s="11">
-        <v>28.1</v>
-      </c>
-      <c r="S33" s="11">
-        <v>38.200000000000003</v>
-      </c>
-      <c r="T33" s="11">
-        <v>31.2</v>
-      </c>
-      <c r="U33" s="11">
-        <v>22</v>
-      </c>
-      <c r="V33" s="11">
-        <v>32.200000000000003</v>
-      </c>
-      <c r="W33" s="11">
-        <v>35.200000000000003</v>
-      </c>
-      <c r="X33" s="11">
-        <v>36.1</v>
-      </c>
-      <c r="Y33" s="11">
-        <v>37.1</v>
-      </c>
-      <c r="Z33" s="11">
-        <v>38.1</v>
-      </c>
-      <c r="AA33" s="11">
-        <v>31.1</v>
-      </c>
-      <c r="AB33" s="11">
-        <v>32.1</v>
-      </c>
-      <c r="AC33" s="11">
-        <v>42</v>
-      </c>
-      <c r="AD33" s="8">
-        <v>99</v>
-      </c>
-      <c r="AE33" s="8">
-        <v>100</v>
-      </c>
-      <c r="AF33" s="8">
-        <v>152</v>
-      </c>
-      <c r="AG33" s="8">
-        <v>154</v>
-      </c>
-      <c r="AH33" s="10">
         <v>160</v>
       </c>
     </row>

</xml_diff>